<commit_message>
Recent commit of Key Management System
</commit_message>
<xml_diff>
--- a/key_distribution.xlsx
+++ b/key_distribution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dagye\OneDrive\Desktop\game\KeyTrack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{921C9924-4B9F-4D32-AE09-7CA5413CB0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9329743C-5FAC-4749-8987-E09654F7156E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14513" yWindow="8108" windowWidth="19396" windowHeight="11474" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -1381,19 +1381,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="88.85546875" customWidth="1"/>
-    <col min="4" max="4" width="70.7109375" customWidth="1"/>
-    <col min="5" max="5" width="65.140625" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="97.19921875" customWidth="1"/>
+    <col min="4" max="4" width="70.73046875" customWidth="1"/>
+    <col min="5" max="5" width="65.1328125" customWidth="1"/>
+    <col min="6" max="6" width="33.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1413,12 +1413,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1427,12 +1427,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1444,7 +1444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>97</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>107</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>111</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>113</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>116</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>119</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>123</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>127</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>132</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>136</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>140</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>146</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>151</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>155</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>160</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>163</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>167</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>169</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>172</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>177</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>180</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>184</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>188</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>193</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>198</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>201</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>203</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>206</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>209</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>213</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>218</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>223</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>225</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>228</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>232</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>236</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>241</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>244</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>248</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>252</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>254</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>256</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>260</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>263</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>267</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>270</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>274</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>276</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>279</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>282</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>285</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>289</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>293</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>296</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>298</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>300</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>303</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>307</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>309</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>313</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>316</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>319</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>321</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>323</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>325</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>328</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>331</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>335</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>339</v>
       </c>

</xml_diff>